<commit_message>
Add department company to report
</commit_message>
<xml_diff>
--- a/front/src/assets/SOLICITAR_CREDITO.xlsx
+++ b/front/src/assets/SOLICITAR_CREDITO.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="127">
   <si>
     <t xml:space="preserve">FONDO DE EMPLEADOS SEAPTO</t>
   </si>
@@ -149,9 +149,6 @@
   </si>
   <si>
     <t>Departamento:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dependencia: COMERCIAL</t>
   </si>
   <si>
     <t xml:space="preserve">Tipo de Contrato</t>
@@ -421,7 +418,7 @@
     <numFmt numFmtId="166" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="167" formatCode="_(&quot;$&quot;\ * #,##0.00_);_(&quot;$&quot;\ * \(#,##0.00\);_(&quot;$&quot;\ * &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="19">
+  <fonts count="18">
     <font>
       <sz val="11.000000"/>
       <color theme="1"/>
@@ -430,56 +427,46 @@
     </font>
     <font>
       <sz val="12.000000"/>
-      <color indexed="64"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
       <sz val="14.000000"/>
-      <color indexed="64"/>
       <name val="Tahoma"/>
     </font>
     <font>
       <b/>
       <sz val="11.000000"/>
-      <color indexed="64"/>
       <name val="Tahoma"/>
     </font>
     <font>
       <b/>
       <sz val="12.000000"/>
-      <color indexed="64"/>
       <name val="Tahoma"/>
     </font>
     <font>
       <sz val="11.000000"/>
-      <color indexed="64"/>
       <name val="Tahoma"/>
     </font>
     <font>
       <sz val="12.000000"/>
-      <color indexed="64"/>
       <name val="Tahoma"/>
     </font>
     <font>
       <sz val="10.000000"/>
-      <color indexed="64"/>
       <name val="Tahoma"/>
     </font>
     <font>
       <b/>
       <sz val="10.000000"/>
-      <color indexed="64"/>
       <name val="Tahoma"/>
     </font>
     <font>
       <sz val="16.000000"/>
-      <color indexed="64"/>
       <name val="Tahoma"/>
     </font>
     <font>
       <sz val="14.000000"/>
-      <color indexed="64"/>
       <name val="Tahoma"/>
     </font>
     <font>
@@ -500,10 +487,6 @@
     <font>
       <sz val="10.000000"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="11.000000"/>
-      <name val="Tahoma"/>
     </font>
     <font>
       <sz val="10.000000"/>
@@ -548,7 +531,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="15">
     <border>
       <left style="none"/>
       <right style="none"/>
@@ -558,11 +541,11 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="none"/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="none"/>
       <diagonal style="none"/>
@@ -570,24 +553,24 @@
     <border>
       <left style="none"/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="none"/>
       <diagonal style="none"/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="none"/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal style="none"/>
     </border>
@@ -595,29 +578,29 @@
       <left style="none"/>
       <right style="none"/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal style="none"/>
     </border>
     <border>
       <left style="none"/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal style="none"/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="none"/>
       <top style="none"/>
@@ -627,91 +610,10 @@
     <border>
       <left style="none"/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="none"/>
       <bottom style="none"/>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="none"/>
-      <top style="none"/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="none"/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="none"/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="none"/>
-      <right style="none"/>
-      <top style="none"/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="none"/>
-      <right style="none"/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="none"/>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="none"/>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="none"/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal style="none"/>
     </border>
     <border>
@@ -729,11 +631,77 @@
       </bottom>
       <diagonal style="none"/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="none"/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="none"/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="234">
+  <cellXfs count="233">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -992,10 +960,10 @@
     <xf fontId="5" fillId="0" borderId="3" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf fontId="5" fillId="0" borderId="15" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="5" fillId="0" borderId="8" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf fontId="5" fillId="0" borderId="15" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="5" fillId="0" borderId="8" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf fontId="5" fillId="0" borderId="5" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1005,9 +973,6 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf fontId="5" fillId="0" borderId="8" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf fontId="5" fillId="0" borderId="8" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf fontId="6" fillId="0" borderId="5" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1025,10 +990,10 @@
     <xf fontId="14" fillId="0" borderId="3" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="15" fillId="0" borderId="4" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="5" fillId="0" borderId="4" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="15" fillId="0" borderId="5" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="5" fillId="0" borderId="5" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf fontId="6" fillId="0" borderId="3" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1259,13 +1224,13 @@
     <xf fontId="11" fillId="0" borderId="10" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="16" fillId="3" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="15" fillId="3" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf fontId="16" fillId="3" borderId="12" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="15" fillId="3" borderId="12" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf fontId="16" fillId="3" borderId="2" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="15" fillId="3" borderId="2" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf fontId="1" fillId="3" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1338,16 +1303,16 @@
     <xf fontId="1" fillId="0" borderId="5" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf fontId="17" fillId="2" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="16" fillId="2" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="17" fillId="2" borderId="12" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="16" fillId="2" borderId="12" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="17" fillId="2" borderId="2" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="16" fillId="2" borderId="2" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="18" fillId="3" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf fontId="17" fillId="3" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf fontId="6" fillId="0" borderId="8" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1470,7 +1435,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>807268</xdr:colOff>
+      <xdr:colOff>807267</xdr:colOff>
       <xdr:row>68</xdr:row>
       <xdr:rowOff>1047749</xdr:rowOff>
     </xdr:to>
@@ -1487,8 +1452,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm flipH="0" flipV="0">
-          <a:off x="11342687" y="22494874"/>
-          <a:ext cx="807268" cy="928687"/>
+          <a:off x="11342687" y="22494873"/>
+          <a:ext cx="807268" cy="928686"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2579,9 +2544,7 @@
       <c r="Y16" s="9"/>
     </row>
     <row r="17" ht="13.5" customHeight="1">
-      <c r="A17" s="82" t="s">
-        <v>43</v>
-      </c>
+      <c r="A17" s="82"/>
       <c r="B17" s="82"/>
       <c r="C17" s="82"/>
       <c r="D17" s="82"/>
@@ -2592,18 +2555,18 @@
       <c r="I17" s="82"/>
       <c r="J17" s="82"/>
       <c r="K17" s="59" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L17" s="59"/>
       <c r="M17" s="59"/>
       <c r="N17" s="59"/>
       <c r="O17" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="P17" s="19"/>
       <c r="Q17" s="83"/>
       <c r="R17" s="84" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="S17" s="84"/>
       <c r="T17" s="84"/>
@@ -2635,7 +2598,7 @@
       <c r="M18" s="68"/>
       <c r="N18" s="68"/>
       <c r="O18" s="19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="P18" s="19"/>
       <c r="Q18" s="86"/>
@@ -2656,130 +2619,130 @@
     </row>
     <row r="19" ht="21.75" customHeight="1">
       <c r="A19" s="60" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B19" s="60"/>
       <c r="C19" s="60" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D19" s="60"/>
       <c r="E19" s="87"/>
       <c r="F19" s="88" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G19" s="89"/>
       <c r="H19" s="90" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I19" s="91"/>
       <c r="J19" s="60" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K19" s="60"/>
       <c r="L19" s="91"/>
       <c r="M19" s="60" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="N19" s="60"/>
       <c r="O19" s="60"/>
-      <c r="P19" s="92"/>
+      <c r="P19" s="89"/>
       <c r="Q19" s="60" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="R19" s="60"/>
       <c r="S19" s="60"/>
-      <c r="T19" s="93"/>
-      <c r="U19" s="93"/>
-      <c r="V19" s="93"/>
-      <c r="W19" s="93"/>
+      <c r="T19" s="92"/>
+      <c r="U19" s="92"/>
+      <c r="V19" s="92"/>
+      <c r="W19" s="92"/>
       <c r="X19" s="9"/>
       <c r="Y19" s="9"/>
     </row>
     <row r="20" ht="29.25" customHeight="1">
       <c r="A20" s="80" t="s">
+        <v>54</v>
+      </c>
+      <c r="B20" s="93"/>
+      <c r="C20" s="94"/>
+      <c r="D20" s="95"/>
+      <c r="E20" s="95"/>
+      <c r="F20" s="95"/>
+      <c r="G20" s="95"/>
+      <c r="H20" s="95"/>
+      <c r="I20" s="95"/>
+      <c r="J20" s="96"/>
+      <c r="K20" s="80" t="s">
         <v>55</v>
       </c>
-      <c r="B20" s="94"/>
-      <c r="C20" s="95"/>
-      <c r="D20" s="96"/>
-      <c r="E20" s="96"/>
-      <c r="F20" s="96"/>
-      <c r="G20" s="96"/>
-      <c r="H20" s="96"/>
-      <c r="I20" s="96"/>
-      <c r="J20" s="97"/>
-      <c r="K20" s="80" t="s">
-        <v>56</v>
-      </c>
       <c r="L20" s="81"/>
-      <c r="M20" s="94"/>
-      <c r="N20" s="98"/>
-      <c r="O20" s="99"/>
-      <c r="P20" s="99"/>
-      <c r="Q20" s="99"/>
-      <c r="R20" s="99"/>
-      <c r="S20" s="99"/>
-      <c r="T20" s="99"/>
-      <c r="U20" s="99"/>
-      <c r="V20" s="99"/>
-      <c r="W20" s="100"/>
+      <c r="M20" s="93"/>
+      <c r="N20" s="97"/>
+      <c r="O20" s="98"/>
+      <c r="P20" s="98"/>
+      <c r="Q20" s="98"/>
+      <c r="R20" s="98"/>
+      <c r="S20" s="98"/>
+      <c r="T20" s="98"/>
+      <c r="U20" s="98"/>
+      <c r="V20" s="98"/>
+      <c r="W20" s="99"/>
       <c r="X20" s="9"/>
       <c r="Y20" s="9"/>
     </row>
     <row r="21" ht="29.25" customHeight="1">
       <c r="A21" s="23" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B21" s="24"/>
       <c r="C21" s="24"/>
       <c r="D21" s="24"/>
       <c r="E21" s="25"/>
-      <c r="F21" s="101"/>
-      <c r="G21" s="102"/>
-      <c r="H21" s="102"/>
-      <c r="I21" s="102"/>
-      <c r="J21" s="103"/>
-      <c r="K21" s="104" t="s">
+      <c r="F21" s="100"/>
+      <c r="G21" s="101"/>
+      <c r="H21" s="101"/>
+      <c r="I21" s="101"/>
+      <c r="J21" s="102"/>
+      <c r="K21" s="103" t="s">
+        <v>57</v>
+      </c>
+      <c r="L21" s="104"/>
+      <c r="M21" s="104"/>
+      <c r="N21" s="58"/>
+      <c r="O21" s="105"/>
+      <c r="P21" s="106"/>
+      <c r="Q21" s="107"/>
+      <c r="R21" s="108" t="s">
         <v>58</v>
       </c>
-      <c r="L21" s="105"/>
-      <c r="M21" s="105"/>
-      <c r="N21" s="58"/>
-      <c r="O21" s="106"/>
-      <c r="P21" s="107"/>
-      <c r="Q21" s="108"/>
-      <c r="R21" s="109" t="s">
-        <v>59</v>
-      </c>
-      <c r="S21" s="110"/>
-      <c r="T21" s="110"/>
-      <c r="U21" s="110"/>
-      <c r="V21" s="110"/>
+      <c r="S21" s="109"/>
+      <c r="T21" s="109"/>
+      <c r="U21" s="109"/>
+      <c r="V21" s="109"/>
       <c r="W21" s="67"/>
       <c r="X21" s="9"/>
       <c r="Y21" s="9"/>
     </row>
     <row r="22" ht="21.75" customHeight="1">
       <c r="A22" s="59" t="s">
+        <v>59</v>
+      </c>
+      <c r="B22" s="60" t="s">
         <v>60</v>
-      </c>
-      <c r="B22" s="60" t="s">
-        <v>61</v>
       </c>
       <c r="C22" s="60"/>
       <c r="D22" s="33"/>
-      <c r="E22" s="111" t="s">
+      <c r="E22" s="110" t="s">
+        <v>61</v>
+      </c>
+      <c r="F22" s="111"/>
+      <c r="G22" s="112"/>
+      <c r="H22" s="113">
+        <v>0</v>
+      </c>
+      <c r="I22" s="114"/>
+      <c r="J22" s="115"/>
+      <c r="K22" s="19" t="s">
         <v>62</v>
-      </c>
-      <c r="F22" s="112"/>
-      <c r="G22" s="113"/>
-      <c r="H22" s="114">
-        <v>0</v>
-      </c>
-      <c r="I22" s="115"/>
-      <c r="J22" s="116"/>
-      <c r="K22" s="19" t="s">
-        <v>63</v>
       </c>
       <c r="L22" s="44"/>
       <c r="M22" s="44"/>
@@ -2799,148 +2762,148 @@
     <row r="23" ht="21.75" customHeight="1">
       <c r="A23" s="59"/>
       <c r="B23" s="60" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C23" s="60"/>
       <c r="D23" s="33"/>
-      <c r="E23" s="111" t="s">
+      <c r="E23" s="110" t="s">
+        <v>64</v>
+      </c>
+      <c r="F23" s="111"/>
+      <c r="G23" s="112"/>
+      <c r="H23" s="113"/>
+      <c r="I23" s="114"/>
+      <c r="J23" s="115"/>
+      <c r="K23" s="19" t="s">
         <v>65</v>
-      </c>
-      <c r="F23" s="112"/>
-      <c r="G23" s="113"/>
-      <c r="H23" s="114"/>
-      <c r="I23" s="115"/>
-      <c r="J23" s="116"/>
-      <c r="K23" s="19" t="s">
-        <v>66</v>
       </c>
       <c r="L23" s="44"/>
       <c r="M23" s="44"/>
       <c r="N23" s="44"/>
       <c r="O23" s="44"/>
-      <c r="P23" s="117"/>
-      <c r="Q23" s="118"/>
-      <c r="R23" s="118"/>
-      <c r="S23" s="118"/>
-      <c r="T23" s="118"/>
-      <c r="U23" s="118"/>
-      <c r="V23" s="118"/>
-      <c r="W23" s="119"/>
+      <c r="P23" s="116"/>
+      <c r="Q23" s="117"/>
+      <c r="R23" s="117"/>
+      <c r="S23" s="117"/>
+      <c r="T23" s="117"/>
+      <c r="U23" s="117"/>
+      <c r="V23" s="117"/>
+      <c r="W23" s="118"/>
       <c r="X23" s="9"/>
       <c r="Y23" s="9"/>
     </row>
     <row r="24" ht="21.75" customHeight="1">
       <c r="A24" s="59"/>
-      <c r="B24" s="120" t="s">
+      <c r="B24" s="119" t="s">
+        <v>66</v>
+      </c>
+      <c r="C24" s="119"/>
+      <c r="D24" s="64"/>
+      <c r="E24" s="110" t="s">
         <v>67</v>
       </c>
-      <c r="C24" s="120"/>
-      <c r="D24" s="64"/>
-      <c r="E24" s="111" t="s">
+      <c r="F24" s="111"/>
+      <c r="G24" s="112"/>
+      <c r="H24" s="113"/>
+      <c r="I24" s="114"/>
+      <c r="J24" s="115"/>
+      <c r="K24" s="44" t="s">
         <v>68</v>
-      </c>
-      <c r="F24" s="112"/>
-      <c r="G24" s="113"/>
-      <c r="H24" s="114"/>
-      <c r="I24" s="115"/>
-      <c r="J24" s="116"/>
-      <c r="K24" s="44" t="s">
-        <v>69</v>
       </c>
       <c r="L24" s="44"/>
       <c r="M24" s="44"/>
       <c r="N24" s="44"/>
-      <c r="O24" s="121"/>
-      <c r="P24" s="122"/>
-      <c r="Q24" s="122"/>
-      <c r="R24" s="122"/>
-      <c r="S24" s="122"/>
-      <c r="T24" s="122"/>
-      <c r="U24" s="122"/>
-      <c r="V24" s="122"/>
-      <c r="W24" s="123"/>
+      <c r="O24" s="120"/>
+      <c r="P24" s="121"/>
+      <c r="Q24" s="121"/>
+      <c r="R24" s="121"/>
+      <c r="S24" s="121"/>
+      <c r="T24" s="121"/>
+      <c r="U24" s="121"/>
+      <c r="V24" s="121"/>
+      <c r="W24" s="122"/>
       <c r="X24" s="9"/>
       <c r="Y24" s="9"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="124" t="s">
+      <c r="A25" s="123" t="s">
+        <v>69</v>
+      </c>
+      <c r="B25" s="124" t="s">
         <v>70</v>
       </c>
-      <c r="B25" s="125" t="s">
+      <c r="C25" s="124"/>
+      <c r="D25" s="124"/>
+      <c r="E25" s="125"/>
+      <c r="F25" s="125"/>
+      <c r="G25" s="125"/>
+      <c r="H25" s="125"/>
+      <c r="I25" s="125"/>
+      <c r="J25" s="125"/>
+      <c r="K25" s="126" t="s">
         <v>71</v>
       </c>
-      <c r="C25" s="125"/>
-      <c r="D25" s="125"/>
-      <c r="E25" s="126"/>
-      <c r="F25" s="126"/>
-      <c r="G25" s="126"/>
-      <c r="H25" s="126"/>
-      <c r="I25" s="126"/>
-      <c r="J25" s="126"/>
-      <c r="K25" s="127" t="s">
+      <c r="L25" s="92"/>
+      <c r="M25" s="19" t="s">
         <v>72</v>
-      </c>
-      <c r="L25" s="93"/>
-      <c r="M25" s="19" t="s">
-        <v>73</v>
       </c>
       <c r="N25" s="19"/>
       <c r="O25" s="19"/>
       <c r="P25" s="57"/>
-      <c r="Q25" s="128" t="s">
+      <c r="Q25" s="127" t="s">
+        <v>73</v>
+      </c>
+      <c r="R25" s="128"/>
+      <c r="S25" s="129"/>
+      <c r="T25" s="129"/>
+      <c r="U25" s="129"/>
+      <c r="V25" s="129"/>
+      <c r="W25" s="130"/>
+      <c r="X25" s="131"/>
+      <c r="Y25" s="9"/>
+    </row>
+    <row r="26" ht="13.5" customHeight="1">
+      <c r="A26" s="123"/>
+      <c r="B26" s="124"/>
+      <c r="C26" s="124"/>
+      <c r="D26" s="124"/>
+      <c r="E26" s="125"/>
+      <c r="F26" s="125"/>
+      <c r="G26" s="125"/>
+      <c r="H26" s="125"/>
+      <c r="I26" s="125"/>
+      <c r="J26" s="125"/>
+      <c r="K26" s="126"/>
+      <c r="L26" s="132"/>
+      <c r="M26" s="19" t="s">
         <v>74</v>
-      </c>
-      <c r="R25" s="129"/>
-      <c r="S25" s="130"/>
-      <c r="T25" s="130"/>
-      <c r="U25" s="130"/>
-      <c r="V25" s="130"/>
-      <c r="W25" s="131"/>
-      <c r="X25" s="132"/>
-      <c r="Y25" s="9"/>
-    </row>
-    <row r="26" ht="13.5" customHeight="1">
-      <c r="A26" s="124"/>
-      <c r="B26" s="125"/>
-      <c r="C26" s="125"/>
-      <c r="D26" s="125"/>
-      <c r="E26" s="126"/>
-      <c r="F26" s="126"/>
-      <c r="G26" s="126"/>
-      <c r="H26" s="126"/>
-      <c r="I26" s="126"/>
-      <c r="J26" s="126"/>
-      <c r="K26" s="127"/>
-      <c r="L26" s="133"/>
-      <c r="M26" s="19" t="s">
-        <v>75</v>
       </c>
       <c r="N26" s="19"/>
       <c r="O26" s="19"/>
       <c r="P26" s="19"/>
-      <c r="Q26" s="134"/>
-      <c r="R26" s="135"/>
-      <c r="S26" s="136"/>
-      <c r="T26" s="136"/>
-      <c r="U26" s="136"/>
-      <c r="V26" s="136"/>
-      <c r="W26" s="137"/>
+      <c r="Q26" s="133"/>
+      <c r="R26" s="134"/>
+      <c r="S26" s="135"/>
+      <c r="T26" s="135"/>
+      <c r="U26" s="135"/>
+      <c r="V26" s="135"/>
+      <c r="W26" s="136"/>
       <c r="X26" s="9"/>
       <c r="Y26" s="9"/>
     </row>
     <row r="27" ht="22.5" customHeight="1">
       <c r="A27" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="B27" s="138"/>
-      <c r="C27" s="138"/>
-      <c r="D27" s="138"/>
-      <c r="E27" s="138"/>
-      <c r="F27" s="138"/>
-      <c r="G27" s="138"/>
-      <c r="H27" s="138"/>
-      <c r="I27" s="138"/>
-      <c r="J27" s="138"/>
+        <v>75</v>
+      </c>
+      <c r="B27" s="137"/>
+      <c r="C27" s="137"/>
+      <c r="D27" s="137"/>
+      <c r="E27" s="137"/>
+      <c r="F27" s="137"/>
+      <c r="G27" s="137"/>
+      <c r="H27" s="137"/>
+      <c r="I27" s="137"/>
+      <c r="J27" s="137"/>
       <c r="K27" s="13"/>
       <c r="L27" s="13"/>
       <c r="M27" s="13"/>
@@ -2958,177 +2921,177 @@
       <c r="Y27" s="9"/>
     </row>
     <row r="28" ht="18" customHeight="1">
-      <c r="A28" s="139" t="s">
+      <c r="A28" s="138" t="s">
+        <v>76</v>
+      </c>
+      <c r="B28" s="139"/>
+      <c r="C28" s="140">
+        <v>0</v>
+      </c>
+      <c r="D28" s="141"/>
+      <c r="E28" s="141"/>
+      <c r="F28" s="141"/>
+      <c r="G28" s="141"/>
+      <c r="H28" s="141"/>
+      <c r="I28" s="142"/>
+      <c r="J28" s="138" t="s">
         <v>77</v>
       </c>
-      <c r="B28" s="140"/>
-      <c r="C28" s="141">
+      <c r="K28" s="143"/>
+      <c r="L28" s="143"/>
+      <c r="M28" s="143"/>
+      <c r="N28" s="139"/>
+      <c r="O28" s="140">
         <v>0</v>
       </c>
-      <c r="D28" s="142"/>
-      <c r="E28" s="142"/>
-      <c r="F28" s="142"/>
-      <c r="G28" s="142"/>
-      <c r="H28" s="142"/>
-      <c r="I28" s="143"/>
-      <c r="J28" s="139" t="s">
-        <v>78</v>
-      </c>
-      <c r="K28" s="144"/>
-      <c r="L28" s="144"/>
-      <c r="M28" s="144"/>
-      <c r="N28" s="140"/>
-      <c r="O28" s="141">
-        <v>0</v>
-      </c>
-      <c r="P28" s="142"/>
-      <c r="Q28" s="142"/>
-      <c r="R28" s="142"/>
-      <c r="S28" s="142"/>
-      <c r="T28" s="142"/>
-      <c r="U28" s="142"/>
-      <c r="V28" s="142"/>
-      <c r="W28" s="143"/>
+      <c r="P28" s="141"/>
+      <c r="Q28" s="141"/>
+      <c r="R28" s="141"/>
+      <c r="S28" s="141"/>
+      <c r="T28" s="141"/>
+      <c r="U28" s="141"/>
+      <c r="V28" s="141"/>
+      <c r="W28" s="142"/>
       <c r="X28" s="9"/>
       <c r="Y28" s="9"/>
     </row>
     <row r="29" ht="24" customHeight="1">
-      <c r="A29" s="145" t="s">
+      <c r="A29" s="144" t="s">
+        <v>78</v>
+      </c>
+      <c r="B29" s="79"/>
+      <c r="C29" s="140">
+        <v>0</v>
+      </c>
+      <c r="D29" s="141"/>
+      <c r="E29" s="141"/>
+      <c r="F29" s="141"/>
+      <c r="G29" s="141"/>
+      <c r="H29" s="141"/>
+      <c r="I29" s="142"/>
+      <c r="J29" s="138" t="s">
         <v>79</v>
       </c>
-      <c r="B29" s="79"/>
-      <c r="C29" s="141">
+      <c r="K29" s="143"/>
+      <c r="L29" s="143"/>
+      <c r="M29" s="143"/>
+      <c r="N29" s="139"/>
+      <c r="O29" s="140">
         <v>0</v>
       </c>
-      <c r="D29" s="142"/>
-      <c r="E29" s="142"/>
-      <c r="F29" s="142"/>
-      <c r="G29" s="142"/>
-      <c r="H29" s="142"/>
-      <c r="I29" s="143"/>
-      <c r="J29" s="139" t="s">
-        <v>80</v>
-      </c>
-      <c r="K29" s="144"/>
-      <c r="L29" s="144"/>
-      <c r="M29" s="144"/>
-      <c r="N29" s="140"/>
-      <c r="O29" s="141">
-        <v>0</v>
-      </c>
-      <c r="P29" s="142"/>
-      <c r="Q29" s="142"/>
-      <c r="R29" s="142"/>
-      <c r="S29" s="142"/>
-      <c r="T29" s="142"/>
-      <c r="U29" s="142"/>
-      <c r="V29" s="142"/>
-      <c r="W29" s="143"/>
+      <c r="P29" s="141"/>
+      <c r="Q29" s="141"/>
+      <c r="R29" s="141"/>
+      <c r="S29" s="141"/>
+      <c r="T29" s="141"/>
+      <c r="U29" s="141"/>
+      <c r="V29" s="141"/>
+      <c r="W29" s="142"/>
       <c r="X29" s="9"/>
       <c r="Y29" s="9"/>
     </row>
     <row r="30" ht="27" customHeight="1">
-      <c r="A30" s="139" t="s">
+      <c r="A30" s="138" t="s">
+        <v>80</v>
+      </c>
+      <c r="B30" s="139"/>
+      <c r="C30" s="140">
+        <v>0</v>
+      </c>
+      <c r="D30" s="141"/>
+      <c r="E30" s="141"/>
+      <c r="F30" s="141"/>
+      <c r="G30" s="141"/>
+      <c r="H30" s="141"/>
+      <c r="I30" s="142"/>
+      <c r="J30" s="138" t="s">
         <v>81</v>
       </c>
-      <c r="B30" s="140"/>
-      <c r="C30" s="141">
+      <c r="K30" s="143"/>
+      <c r="L30" s="143"/>
+      <c r="M30" s="143"/>
+      <c r="N30" s="139"/>
+      <c r="O30" s="140">
         <v>0</v>
       </c>
-      <c r="D30" s="142"/>
-      <c r="E30" s="142"/>
-      <c r="F30" s="142"/>
-      <c r="G30" s="142"/>
-      <c r="H30" s="142"/>
-      <c r="I30" s="143"/>
-      <c r="J30" s="139" t="s">
-        <v>82</v>
-      </c>
-      <c r="K30" s="144"/>
-      <c r="L30" s="144"/>
-      <c r="M30" s="144"/>
-      <c r="N30" s="140"/>
-      <c r="O30" s="141">
-        <v>0</v>
-      </c>
-      <c r="P30" s="142"/>
-      <c r="Q30" s="142"/>
-      <c r="R30" s="142"/>
-      <c r="S30" s="142"/>
-      <c r="T30" s="142"/>
-      <c r="U30" s="142"/>
-      <c r="V30" s="142"/>
-      <c r="W30" s="143"/>
+      <c r="P30" s="141"/>
+      <c r="Q30" s="141"/>
+      <c r="R30" s="141"/>
+      <c r="S30" s="141"/>
+      <c r="T30" s="141"/>
+      <c r="U30" s="141"/>
+      <c r="V30" s="141"/>
+      <c r="W30" s="142"/>
       <c r="X30" s="9"/>
       <c r="Y30" s="9"/>
     </row>
     <row r="31" ht="16.5">
-      <c r="A31" s="146" t="s">
-        <v>83</v>
-      </c>
-      <c r="B31" s="147"/>
-      <c r="C31" s="141">
+      <c r="A31" s="145" t="s">
+        <v>82</v>
+      </c>
+      <c r="B31" s="146"/>
+      <c r="C31" s="140">
         <f>SUM(C28:I30)</f>
         <v>0</v>
       </c>
-      <c r="D31" s="142"/>
-      <c r="E31" s="142"/>
-      <c r="F31" s="142"/>
-      <c r="G31" s="142"/>
-      <c r="H31" s="142"/>
-      <c r="I31" s="143"/>
-      <c r="J31" s="146" t="s">
-        <v>84</v>
-      </c>
-      <c r="K31" s="148"/>
-      <c r="L31" s="148"/>
-      <c r="M31" s="148"/>
-      <c r="N31" s="147"/>
-      <c r="O31" s="141">
+      <c r="D31" s="141"/>
+      <c r="E31" s="141"/>
+      <c r="F31" s="141"/>
+      <c r="G31" s="141"/>
+      <c r="H31" s="141"/>
+      <c r="I31" s="142"/>
+      <c r="J31" s="145" t="s">
+        <v>83</v>
+      </c>
+      <c r="K31" s="147"/>
+      <c r="L31" s="147"/>
+      <c r="M31" s="147"/>
+      <c r="N31" s="146"/>
+      <c r="O31" s="140">
         <f>SUM(O28:W30)</f>
         <v>0</v>
       </c>
-      <c r="P31" s="142"/>
-      <c r="Q31" s="142"/>
-      <c r="R31" s="142"/>
-      <c r="S31" s="142"/>
-      <c r="T31" s="142"/>
-      <c r="U31" s="142"/>
-      <c r="V31" s="142"/>
-      <c r="W31" s="143"/>
+      <c r="P31" s="141"/>
+      <c r="Q31" s="141"/>
+      <c r="R31" s="141"/>
+      <c r="S31" s="141"/>
+      <c r="T31" s="141"/>
+      <c r="U31" s="141"/>
+      <c r="V31" s="141"/>
+      <c r="W31" s="142"/>
       <c r="X31" s="9"/>
       <c r="Y31" s="9"/>
     </row>
     <row r="32" ht="16.5">
-      <c r="A32" s="149" t="s">
+      <c r="A32" s="148" t="s">
+        <v>84</v>
+      </c>
+      <c r="B32" s="149"/>
+      <c r="C32" s="150"/>
+      <c r="D32" s="151"/>
+      <c r="E32" s="151"/>
+      <c r="F32" s="151"/>
+      <c r="G32" s="151"/>
+      <c r="H32" s="151"/>
+      <c r="I32" s="152"/>
+      <c r="J32" s="145" t="s">
         <v>85</v>
       </c>
-      <c r="B32" s="150"/>
-      <c r="C32" s="151"/>
-      <c r="D32" s="152"/>
-      <c r="E32" s="152"/>
-      <c r="F32" s="152"/>
-      <c r="G32" s="152"/>
-      <c r="H32" s="152"/>
-      <c r="I32" s="153"/>
-      <c r="J32" s="146" t="s">
-        <v>86</v>
-      </c>
-      <c r="K32" s="148"/>
-      <c r="L32" s="148"/>
-      <c r="M32" s="148"/>
-      <c r="N32" s="147"/>
-      <c r="O32" s="141">
+      <c r="K32" s="147"/>
+      <c r="L32" s="147"/>
+      <c r="M32" s="147"/>
+      <c r="N32" s="146"/>
+      <c r="O32" s="140">
         <v>0</v>
       </c>
-      <c r="P32" s="142"/>
-      <c r="Q32" s="142"/>
-      <c r="R32" s="142"/>
-      <c r="S32" s="142"/>
-      <c r="T32" s="142"/>
-      <c r="U32" s="142"/>
-      <c r="V32" s="142"/>
-      <c r="W32" s="143"/>
+      <c r="P32" s="141"/>
+      <c r="Q32" s="141"/>
+      <c r="R32" s="141"/>
+      <c r="S32" s="141"/>
+      <c r="T32" s="141"/>
+      <c r="U32" s="141"/>
+      <c r="V32" s="141"/>
+      <c r="W32" s="142"/>
       <c r="X32" s="9"/>
       <c r="Y32" s="9"/>
     </row>
@@ -3142,62 +3105,62 @@
       <c r="G33" s="24"/>
       <c r="H33" s="24"/>
       <c r="I33" s="25"/>
-      <c r="J33" s="148" t="s">
-        <v>87</v>
-      </c>
-      <c r="K33" s="148"/>
-      <c r="L33" s="148"/>
-      <c r="M33" s="148"/>
-      <c r="N33" s="147"/>
-      <c r="O33" s="141">
+      <c r="J33" s="147" t="s">
+        <v>86</v>
+      </c>
+      <c r="K33" s="147"/>
+      <c r="L33" s="147"/>
+      <c r="M33" s="147"/>
+      <c r="N33" s="146"/>
+      <c r="O33" s="140">
         <v>0</v>
       </c>
-      <c r="P33" s="142"/>
-      <c r="Q33" s="142"/>
-      <c r="R33" s="142"/>
-      <c r="S33" s="142"/>
-      <c r="T33" s="142"/>
-      <c r="U33" s="142"/>
-      <c r="V33" s="142"/>
-      <c r="W33" s="143"/>
+      <c r="P33" s="141"/>
+      <c r="Q33" s="141"/>
+      <c r="R33" s="141"/>
+      <c r="S33" s="141"/>
+      <c r="T33" s="141"/>
+      <c r="U33" s="141"/>
+      <c r="V33" s="141"/>
+      <c r="W33" s="142"/>
       <c r="X33" s="9"/>
       <c r="Y33" s="9"/>
     </row>
     <row r="34" ht="16.5">
-      <c r="A34" s="154"/>
-      <c r="B34" s="155"/>
-      <c r="C34" s="155"/>
-      <c r="D34" s="155"/>
-      <c r="E34" s="155"/>
-      <c r="F34" s="155"/>
-      <c r="G34" s="155"/>
-      <c r="H34" s="155"/>
-      <c r="I34" s="156"/>
-      <c r="J34" s="157" t="s">
-        <v>88</v>
-      </c>
-      <c r="K34" s="158"/>
-      <c r="L34" s="158"/>
-      <c r="M34" s="158"/>
-      <c r="N34" s="159"/>
-      <c r="O34" s="151">
+      <c r="A34" s="153"/>
+      <c r="B34" s="154"/>
+      <c r="C34" s="154"/>
+      <c r="D34" s="154"/>
+      <c r="E34" s="154"/>
+      <c r="F34" s="154"/>
+      <c r="G34" s="154"/>
+      <c r="H34" s="154"/>
+      <c r="I34" s="155"/>
+      <c r="J34" s="156" t="s">
+        <v>87</v>
+      </c>
+      <c r="K34" s="157"/>
+      <c r="L34" s="157"/>
+      <c r="M34" s="157"/>
+      <c r="N34" s="158"/>
+      <c r="O34" s="150">
         <f>O32-O33</f>
         <v>0</v>
       </c>
-      <c r="P34" s="152"/>
-      <c r="Q34" s="152"/>
-      <c r="R34" s="152"/>
-      <c r="S34" s="152"/>
-      <c r="T34" s="152"/>
-      <c r="U34" s="152"/>
-      <c r="V34" s="152"/>
-      <c r="W34" s="153"/>
+      <c r="P34" s="151"/>
+      <c r="Q34" s="151"/>
+      <c r="R34" s="151"/>
+      <c r="S34" s="151"/>
+      <c r="T34" s="151"/>
+      <c r="U34" s="151"/>
+      <c r="V34" s="151"/>
+      <c r="W34" s="152"/>
       <c r="X34" s="9"/>
       <c r="Y34" s="9"/>
     </row>
     <row r="35" ht="22.5" customHeight="1">
       <c r="A35" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B35" s="13"/>
       <c r="C35" s="13"/>
@@ -3226,7 +3189,7 @@
     </row>
     <row r="36" ht="16.5">
       <c r="A36" s="19" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B36" s="19"/>
       <c r="C36" s="57"/>
@@ -3236,7 +3199,7 @@
       <c r="G36" s="57"/>
       <c r="H36" s="57"/>
       <c r="I36" s="19" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J36" s="19"/>
       <c r="K36" s="19"/>
@@ -3244,16 +3207,16 @@
       <c r="M36" s="57"/>
       <c r="N36" s="57"/>
       <c r="O36" s="44" t="s">
-        <v>92</v>
-      </c>
-      <c r="P36" s="160"/>
-      <c r="Q36" s="160"/>
-      <c r="R36" s="160"/>
-      <c r="S36" s="160"/>
-      <c r="T36" s="160"/>
-      <c r="U36" s="160"/>
-      <c r="V36" s="160"/>
-      <c r="W36" s="160"/>
+        <v>91</v>
+      </c>
+      <c r="P36" s="159"/>
+      <c r="Q36" s="159"/>
+      <c r="R36" s="159"/>
+      <c r="S36" s="159"/>
+      <c r="T36" s="159"/>
+      <c r="U36" s="159"/>
+      <c r="V36" s="159"/>
+      <c r="W36" s="159"/>
       <c r="X36" s="9"/>
       <c r="Y36" s="9"/>
     </row>
@@ -3269,30 +3232,30 @@
       <c r="G37" s="57"/>
       <c r="H37" s="57"/>
       <c r="I37" s="19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J37" s="19"/>
       <c r="K37" s="19"/>
       <c r="L37" s="57"/>
       <c r="M37" s="57"/>
       <c r="N37" s="57"/>
-      <c r="O37" s="161" t="s">
-        <v>94</v>
-      </c>
-      <c r="P37" s="162"/>
-      <c r="Q37" s="162"/>
-      <c r="R37" s="162"/>
-      <c r="S37" s="162"/>
-      <c r="T37" s="162"/>
-      <c r="U37" s="162"/>
-      <c r="V37" s="162"/>
-      <c r="W37" s="162"/>
+      <c r="O37" s="160" t="s">
+        <v>93</v>
+      </c>
+      <c r="P37" s="161"/>
+      <c r="Q37" s="161"/>
+      <c r="R37" s="161"/>
+      <c r="S37" s="161"/>
+      <c r="T37" s="161"/>
+      <c r="U37" s="161"/>
+      <c r="V37" s="161"/>
+      <c r="W37" s="161"/>
       <c r="X37" s="9"/>
       <c r="Y37" s="9"/>
     </row>
     <row r="38" ht="22.5" customHeight="1">
       <c r="A38" s="12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B38" s="13"/>
       <c r="C38" s="13"/>
@@ -3321,7 +3284,7 @@
     </row>
     <row r="39" ht="16.5">
       <c r="A39" s="19" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B39" s="19"/>
       <c r="C39" s="57"/>
@@ -3331,7 +3294,7 @@
       <c r="G39" s="57"/>
       <c r="H39" s="57"/>
       <c r="I39" s="19" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J39" s="19"/>
       <c r="K39" s="19"/>
@@ -3339,16 +3302,16 @@
       <c r="M39" s="57"/>
       <c r="N39" s="57"/>
       <c r="O39" s="44" t="s">
-        <v>92</v>
-      </c>
-      <c r="P39" s="160"/>
-      <c r="Q39" s="160"/>
-      <c r="R39" s="160"/>
-      <c r="S39" s="160"/>
-      <c r="T39" s="160"/>
-      <c r="U39" s="160"/>
-      <c r="V39" s="160"/>
-      <c r="W39" s="160"/>
+        <v>91</v>
+      </c>
+      <c r="P39" s="159"/>
+      <c r="Q39" s="159"/>
+      <c r="R39" s="159"/>
+      <c r="S39" s="159"/>
+      <c r="T39" s="159"/>
+      <c r="U39" s="159"/>
+      <c r="V39" s="159"/>
+      <c r="W39" s="159"/>
       <c r="X39" s="9"/>
       <c r="Y39" s="9"/>
     </row>
@@ -3364,30 +3327,30 @@
       <c r="G40" s="57"/>
       <c r="H40" s="57"/>
       <c r="I40" s="19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J40" s="19"/>
       <c r="K40" s="19"/>
       <c r="L40" s="57"/>
       <c r="M40" s="57"/>
       <c r="N40" s="57"/>
-      <c r="O40" s="161" t="s">
-        <v>94</v>
-      </c>
-      <c r="P40" s="162"/>
-      <c r="Q40" s="162"/>
-      <c r="R40" s="162"/>
-      <c r="S40" s="162"/>
-      <c r="T40" s="162"/>
-      <c r="U40" s="162"/>
-      <c r="V40" s="162"/>
-      <c r="W40" s="162"/>
+      <c r="O40" s="160" t="s">
+        <v>93</v>
+      </c>
+      <c r="P40" s="161"/>
+      <c r="Q40" s="161"/>
+      <c r="R40" s="161"/>
+      <c r="S40" s="161"/>
+      <c r="T40" s="161"/>
+      <c r="U40" s="161"/>
+      <c r="V40" s="161"/>
+      <c r="W40" s="161"/>
       <c r="X40" s="9"/>
       <c r="Y40" s="9"/>
     </row>
     <row r="41" ht="22.5" customHeight="1">
       <c r="A41" s="12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B41" s="13"/>
       <c r="C41" s="13"/>
@@ -3415,473 +3378,473 @@
       <c r="Y41" s="9"/>
     </row>
     <row r="42" ht="99.75" customHeight="1">
-      <c r="A42" s="163" t="s">
-        <v>97</v>
-      </c>
-      <c r="B42" s="164"/>
-      <c r="C42" s="164"/>
-      <c r="D42" s="164"/>
-      <c r="E42" s="164"/>
-      <c r="F42" s="164"/>
-      <c r="G42" s="164"/>
-      <c r="H42" s="164"/>
-      <c r="I42" s="164"/>
-      <c r="J42" s="164"/>
-      <c r="K42" s="164"/>
-      <c r="L42" s="164"/>
-      <c r="M42" s="164"/>
-      <c r="N42" s="164"/>
-      <c r="O42" s="164"/>
-      <c r="P42" s="164"/>
-      <c r="Q42" s="164"/>
-      <c r="R42" s="164"/>
-      <c r="S42" s="164"/>
-      <c r="T42" s="164"/>
-      <c r="U42" s="164"/>
-      <c r="V42" s="164"/>
-      <c r="W42" s="165"/>
+      <c r="A42" s="162" t="s">
+        <v>96</v>
+      </c>
+      <c r="B42" s="163"/>
+      <c r="C42" s="163"/>
+      <c r="D42" s="163"/>
+      <c r="E42" s="163"/>
+      <c r="F42" s="163"/>
+      <c r="G42" s="163"/>
+      <c r="H42" s="163"/>
+      <c r="I42" s="163"/>
+      <c r="J42" s="163"/>
+      <c r="K42" s="163"/>
+      <c r="L42" s="163"/>
+      <c r="M42" s="163"/>
+      <c r="N42" s="163"/>
+      <c r="O42" s="163"/>
+      <c r="P42" s="163"/>
+      <c r="Q42" s="163"/>
+      <c r="R42" s="163"/>
+      <c r="S42" s="163"/>
+      <c r="T42" s="163"/>
+      <c r="U42" s="163"/>
+      <c r="V42" s="163"/>
+      <c r="W42" s="164"/>
       <c r="X42" s="9"/>
       <c r="Y42" s="9"/>
     </row>
     <row r="43" ht="22.5" customHeight="1">
-      <c r="A43" s="166" t="s">
-        <v>98</v>
-      </c>
-      <c r="B43" s="166"/>
-      <c r="C43" s="166"/>
-      <c r="D43" s="166"/>
-      <c r="E43" s="166"/>
-      <c r="F43" s="166"/>
-      <c r="G43" s="166"/>
-      <c r="H43" s="166"/>
-      <c r="I43" s="166"/>
-      <c r="J43" s="166"/>
-      <c r="K43" s="166"/>
-      <c r="L43" s="166"/>
-      <c r="M43" s="166"/>
-      <c r="N43" s="166"/>
-      <c r="O43" s="166"/>
-      <c r="P43" s="166"/>
-      <c r="Q43" s="166"/>
-      <c r="R43" s="166"/>
-      <c r="S43" s="166"/>
-      <c r="T43" s="166"/>
-      <c r="U43" s="166"/>
-      <c r="V43" s="166"/>
-      <c r="W43" s="166"/>
+      <c r="A43" s="165" t="s">
+        <v>97</v>
+      </c>
+      <c r="B43" s="165"/>
+      <c r="C43" s="165"/>
+      <c r="D43" s="165"/>
+      <c r="E43" s="165"/>
+      <c r="F43" s="165"/>
+      <c r="G43" s="165"/>
+      <c r="H43" s="165"/>
+      <c r="I43" s="165"/>
+      <c r="J43" s="165"/>
+      <c r="K43" s="165"/>
+      <c r="L43" s="165"/>
+      <c r="M43" s="165"/>
+      <c r="N43" s="165"/>
+      <c r="O43" s="165"/>
+      <c r="P43" s="165"/>
+      <c r="Q43" s="165"/>
+      <c r="R43" s="165"/>
+      <c r="S43" s="165"/>
+      <c r="T43" s="165"/>
+      <c r="U43" s="165"/>
+      <c r="V43" s="165"/>
+      <c r="W43" s="165"/>
       <c r="X43" s="9"/>
       <c r="Y43" s="9"/>
     </row>
     <row r="44" ht="38.25" customHeight="1">
-      <c r="A44" s="167" t="s">
-        <v>99</v>
-      </c>
-      <c r="B44" s="168"/>
-      <c r="C44" s="168"/>
-      <c r="D44" s="168"/>
-      <c r="E44" s="168"/>
-      <c r="F44" s="168"/>
-      <c r="G44" s="168"/>
-      <c r="H44" s="168"/>
-      <c r="I44" s="168"/>
-      <c r="J44" s="168"/>
-      <c r="K44" s="168"/>
-      <c r="L44" s="168"/>
-      <c r="M44" s="168"/>
-      <c r="N44" s="168"/>
-      <c r="O44" s="168"/>
-      <c r="P44" s="168"/>
-      <c r="Q44" s="168"/>
-      <c r="R44" s="168"/>
-      <c r="S44" s="168"/>
-      <c r="T44" s="168"/>
-      <c r="U44" s="168"/>
-      <c r="V44" s="168"/>
-      <c r="W44" s="169"/>
+      <c r="A44" s="166" t="s">
+        <v>98</v>
+      </c>
+      <c r="B44" s="167"/>
+      <c r="C44" s="167"/>
+      <c r="D44" s="167"/>
+      <c r="E44" s="167"/>
+      <c r="F44" s="167"/>
+      <c r="G44" s="167"/>
+      <c r="H44" s="167"/>
+      <c r="I44" s="167"/>
+      <c r="J44" s="167"/>
+      <c r="K44" s="167"/>
+      <c r="L44" s="167"/>
+      <c r="M44" s="167"/>
+      <c r="N44" s="167"/>
+      <c r="O44" s="167"/>
+      <c r="P44" s="167"/>
+      <c r="Q44" s="167"/>
+      <c r="R44" s="167"/>
+      <c r="S44" s="167"/>
+      <c r="T44" s="167"/>
+      <c r="U44" s="167"/>
+      <c r="V44" s="167"/>
+      <c r="W44" s="168"/>
       <c r="X44" s="9"/>
       <c r="Y44" s="9"/>
     </row>
     <row r="45" ht="114.75" customHeight="1">
-      <c r="A45" s="170" t="s">
-        <v>100</v>
-      </c>
-      <c r="B45" s="171"/>
-      <c r="C45" s="171"/>
-      <c r="D45" s="171"/>
-      <c r="E45" s="171"/>
-      <c r="F45" s="171"/>
-      <c r="G45" s="171"/>
-      <c r="H45" s="171"/>
-      <c r="I45" s="171"/>
-      <c r="J45" s="171"/>
-      <c r="K45" s="171"/>
-      <c r="L45" s="171"/>
-      <c r="M45" s="171"/>
-      <c r="N45" s="171"/>
-      <c r="O45" s="171"/>
-      <c r="P45" s="171"/>
-      <c r="Q45" s="171"/>
-      <c r="R45" s="171"/>
-      <c r="S45" s="171"/>
-      <c r="T45" s="171"/>
-      <c r="U45" s="171"/>
-      <c r="V45" s="171"/>
-      <c r="W45" s="172"/>
+      <c r="A45" s="169" t="s">
+        <v>99</v>
+      </c>
+      <c r="B45" s="170"/>
+      <c r="C45" s="170"/>
+      <c r="D45" s="170"/>
+      <c r="E45" s="170"/>
+      <c r="F45" s="170"/>
+      <c r="G45" s="170"/>
+      <c r="H45" s="170"/>
+      <c r="I45" s="170"/>
+      <c r="J45" s="170"/>
+      <c r="K45" s="170"/>
+      <c r="L45" s="170"/>
+      <c r="M45" s="170"/>
+      <c r="N45" s="170"/>
+      <c r="O45" s="170"/>
+      <c r="P45" s="170"/>
+      <c r="Q45" s="170"/>
+      <c r="R45" s="170"/>
+      <c r="S45" s="170"/>
+      <c r="T45" s="170"/>
+      <c r="U45" s="170"/>
+      <c r="V45" s="170"/>
+      <c r="W45" s="171"/>
       <c r="X45" s="9"/>
       <c r="Y45" s="9"/>
     </row>
     <row r="46" ht="39.75" customHeight="1">
-      <c r="A46" s="173" t="s">
-        <v>101</v>
-      </c>
-      <c r="B46" s="174"/>
-      <c r="C46" s="174"/>
-      <c r="D46" s="174"/>
-      <c r="E46" s="174"/>
-      <c r="F46" s="174"/>
-      <c r="G46" s="174"/>
-      <c r="H46" s="174"/>
-      <c r="I46" s="174"/>
-      <c r="J46" s="174"/>
-      <c r="K46" s="174"/>
-      <c r="L46" s="174"/>
-      <c r="M46" s="174"/>
-      <c r="N46" s="174"/>
-      <c r="O46" s="174"/>
-      <c r="P46" s="174"/>
-      <c r="Q46" s="174"/>
-      <c r="R46" s="174"/>
-      <c r="S46" s="174"/>
-      <c r="T46" s="174"/>
-      <c r="U46" s="174"/>
-      <c r="V46" s="174"/>
-      <c r="W46" s="175"/>
+      <c r="A46" s="172" t="s">
+        <v>100</v>
+      </c>
+      <c r="B46" s="173"/>
+      <c r="C46" s="173"/>
+      <c r="D46" s="173"/>
+      <c r="E46" s="173"/>
+      <c r="F46" s="173"/>
+      <c r="G46" s="173"/>
+      <c r="H46" s="173"/>
+      <c r="I46" s="173"/>
+      <c r="J46" s="173"/>
+      <c r="K46" s="173"/>
+      <c r="L46" s="173"/>
+      <c r="M46" s="173"/>
+      <c r="N46" s="173"/>
+      <c r="O46" s="173"/>
+      <c r="P46" s="173"/>
+      <c r="Q46" s="173"/>
+      <c r="R46" s="173"/>
+      <c r="S46" s="173"/>
+      <c r="T46" s="173"/>
+      <c r="U46" s="173"/>
+      <c r="V46" s="173"/>
+      <c r="W46" s="174"/>
       <c r="X46" s="9"/>
       <c r="Y46" s="9"/>
     </row>
     <row r="47" ht="22.5" customHeight="1">
-      <c r="A47" s="166" t="s">
-        <v>102</v>
-      </c>
-      <c r="B47" s="166"/>
-      <c r="C47" s="166"/>
-      <c r="D47" s="166"/>
-      <c r="E47" s="166"/>
-      <c r="F47" s="166"/>
-      <c r="G47" s="166"/>
-      <c r="H47" s="166"/>
-      <c r="I47" s="166"/>
-      <c r="J47" s="166"/>
-      <c r="K47" s="166"/>
-      <c r="L47" s="166"/>
-      <c r="M47" s="166"/>
-      <c r="N47" s="166"/>
-      <c r="O47" s="166"/>
-      <c r="P47" s="166"/>
-      <c r="Q47" s="166"/>
-      <c r="R47" s="166"/>
-      <c r="S47" s="166"/>
-      <c r="T47" s="166"/>
-      <c r="U47" s="166"/>
-      <c r="V47" s="166"/>
-      <c r="W47" s="166"/>
+      <c r="A47" s="165" t="s">
+        <v>101</v>
+      </c>
+      <c r="B47" s="165"/>
+      <c r="C47" s="165"/>
+      <c r="D47" s="165"/>
+      <c r="E47" s="165"/>
+      <c r="F47" s="165"/>
+      <c r="G47" s="165"/>
+      <c r="H47" s="165"/>
+      <c r="I47" s="165"/>
+      <c r="J47" s="165"/>
+      <c r="K47" s="165"/>
+      <c r="L47" s="165"/>
+      <c r="M47" s="165"/>
+      <c r="N47" s="165"/>
+      <c r="O47" s="165"/>
+      <c r="P47" s="165"/>
+      <c r="Q47" s="165"/>
+      <c r="R47" s="165"/>
+      <c r="S47" s="165"/>
+      <c r="T47" s="165"/>
+      <c r="U47" s="165"/>
+      <c r="V47" s="165"/>
+      <c r="W47" s="165"/>
       <c r="X47" s="9"/>
       <c r="Y47" s="9"/>
     </row>
     <row r="48" ht="75" customHeight="1">
-      <c r="A48" s="176" t="s">
-        <v>103</v>
-      </c>
-      <c r="B48" s="177"/>
-      <c r="C48" s="177"/>
-      <c r="D48" s="177"/>
-      <c r="E48" s="177"/>
-      <c r="F48" s="177"/>
-      <c r="G48" s="177"/>
-      <c r="H48" s="177"/>
-      <c r="I48" s="177"/>
-      <c r="J48" s="177"/>
-      <c r="K48" s="177"/>
-      <c r="L48" s="177"/>
-      <c r="M48" s="177"/>
-      <c r="N48" s="177"/>
-      <c r="O48" s="177"/>
-      <c r="P48" s="177"/>
-      <c r="Q48" s="177"/>
-      <c r="R48" s="177"/>
-      <c r="S48" s="177"/>
-      <c r="T48" s="177"/>
-      <c r="U48" s="177"/>
-      <c r="V48" s="177"/>
-      <c r="W48" s="178"/>
+      <c r="A48" s="175" t="s">
+        <v>102</v>
+      </c>
+      <c r="B48" s="176"/>
+      <c r="C48" s="176"/>
+      <c r="D48" s="176"/>
+      <c r="E48" s="176"/>
+      <c r="F48" s="176"/>
+      <c r="G48" s="176"/>
+      <c r="H48" s="176"/>
+      <c r="I48" s="176"/>
+      <c r="J48" s="176"/>
+      <c r="K48" s="176"/>
+      <c r="L48" s="176"/>
+      <c r="M48" s="176"/>
+      <c r="N48" s="176"/>
+      <c r="O48" s="176"/>
+      <c r="P48" s="176"/>
+      <c r="Q48" s="176"/>
+      <c r="R48" s="176"/>
+      <c r="S48" s="176"/>
+      <c r="T48" s="176"/>
+      <c r="U48" s="176"/>
+      <c r="V48" s="176"/>
+      <c r="W48" s="177"/>
       <c r="X48" s="9"/>
       <c r="Y48" s="9"/>
     </row>
     <row r="49" ht="107.25" customHeight="1">
-      <c r="A49" s="179" t="s">
-        <v>104</v>
-      </c>
-      <c r="B49" s="180"/>
-      <c r="C49" s="180"/>
-      <c r="D49" s="180"/>
-      <c r="E49" s="180"/>
-      <c r="F49" s="180"/>
-      <c r="G49" s="180"/>
-      <c r="H49" s="180"/>
-      <c r="I49" s="180"/>
-      <c r="J49" s="180"/>
-      <c r="K49" s="180"/>
-      <c r="L49" s="180"/>
-      <c r="M49" s="180"/>
-      <c r="N49" s="180"/>
-      <c r="O49" s="181"/>
-      <c r="P49" s="182"/>
-      <c r="Q49" s="183"/>
-      <c r="R49" s="183"/>
-      <c r="S49" s="183"/>
-      <c r="T49" s="184"/>
-      <c r="U49" s="184"/>
-      <c r="V49" s="184"/>
-      <c r="W49" s="185"/>
+      <c r="A49" s="178" t="s">
+        <v>103</v>
+      </c>
+      <c r="B49" s="179"/>
+      <c r="C49" s="179"/>
+      <c r="D49" s="179"/>
+      <c r="E49" s="179"/>
+      <c r="F49" s="179"/>
+      <c r="G49" s="179"/>
+      <c r="H49" s="179"/>
+      <c r="I49" s="179"/>
+      <c r="J49" s="179"/>
+      <c r="K49" s="179"/>
+      <c r="L49" s="179"/>
+      <c r="M49" s="179"/>
+      <c r="N49" s="179"/>
+      <c r="O49" s="180"/>
+      <c r="P49" s="181"/>
+      <c r="Q49" s="182"/>
+      <c r="R49" s="182"/>
+      <c r="S49" s="182"/>
+      <c r="T49" s="183"/>
+      <c r="U49" s="183"/>
+      <c r="V49" s="183"/>
+      <c r="W49" s="184"/>
       <c r="X49" s="9"/>
       <c r="Y49" s="9"/>
     </row>
     <row r="50" ht="34.5" customHeight="1">
-      <c r="A50" s="186" t="s">
+      <c r="A50" s="185" t="s">
+        <v>104</v>
+      </c>
+      <c r="B50" s="186"/>
+      <c r="C50" s="186"/>
+      <c r="D50" s="186"/>
+      <c r="E50" s="186"/>
+      <c r="F50" s="186"/>
+      <c r="G50" s="186"/>
+      <c r="H50" s="186"/>
+      <c r="I50" s="186"/>
+      <c r="J50" s="186"/>
+      <c r="K50" s="186"/>
+      <c r="L50" s="186"/>
+      <c r="M50" s="186"/>
+      <c r="N50" s="186"/>
+      <c r="O50" s="187"/>
+      <c r="P50" s="188" t="s">
         <v>105</v>
       </c>
-      <c r="B50" s="187"/>
-      <c r="C50" s="187"/>
-      <c r="D50" s="187"/>
-      <c r="E50" s="187"/>
-      <c r="F50" s="187"/>
-      <c r="G50" s="187"/>
-      <c r="H50" s="187"/>
-      <c r="I50" s="187"/>
-      <c r="J50" s="187"/>
-      <c r="K50" s="187"/>
-      <c r="L50" s="187"/>
-      <c r="M50" s="187"/>
-      <c r="N50" s="187"/>
-      <c r="O50" s="188"/>
-      <c r="P50" s="189" t="s">
-        <v>106</v>
-      </c>
-      <c r="Q50" s="190"/>
-      <c r="R50" s="190"/>
-      <c r="S50" s="190"/>
-      <c r="T50" s="190"/>
-      <c r="U50" s="190"/>
-      <c r="V50" s="190"/>
-      <c r="W50" s="191"/>
+      <c r="Q50" s="189"/>
+      <c r="R50" s="189"/>
+      <c r="S50" s="189"/>
+      <c r="T50" s="189"/>
+      <c r="U50" s="189"/>
+      <c r="V50" s="189"/>
+      <c r="W50" s="190"/>
       <c r="X50" s="9"/>
       <c r="Y50" s="9"/>
     </row>
     <row r="51" ht="31.5" customHeight="1">
-      <c r="A51" s="192" t="s">
-        <v>107</v>
-      </c>
-      <c r="B51" s="193"/>
-      <c r="C51" s="193"/>
-      <c r="D51" s="193"/>
-      <c r="E51" s="193"/>
-      <c r="F51" s="193"/>
-      <c r="G51" s="193"/>
-      <c r="H51" s="193"/>
-      <c r="I51" s="193"/>
-      <c r="J51" s="193"/>
-      <c r="K51" s="193"/>
-      <c r="L51" s="193"/>
-      <c r="M51" s="193"/>
-      <c r="N51" s="193"/>
-      <c r="O51" s="193"/>
-      <c r="P51" s="193"/>
-      <c r="Q51" s="193"/>
-      <c r="R51" s="193"/>
-      <c r="S51" s="193"/>
-      <c r="T51" s="193"/>
-      <c r="U51" s="193"/>
-      <c r="V51" s="193"/>
-      <c r="W51" s="194"/>
+      <c r="A51" s="191" t="s">
+        <v>106</v>
+      </c>
+      <c r="B51" s="192"/>
+      <c r="C51" s="192"/>
+      <c r="D51" s="192"/>
+      <c r="E51" s="192"/>
+      <c r="F51" s="192"/>
+      <c r="G51" s="192"/>
+      <c r="H51" s="192"/>
+      <c r="I51" s="192"/>
+      <c r="J51" s="192"/>
+      <c r="K51" s="192"/>
+      <c r="L51" s="192"/>
+      <c r="M51" s="192"/>
+      <c r="N51" s="192"/>
+      <c r="O51" s="192"/>
+      <c r="P51" s="192"/>
+      <c r="Q51" s="192"/>
+      <c r="R51" s="192"/>
+      <c r="S51" s="192"/>
+      <c r="T51" s="192"/>
+      <c r="U51" s="192"/>
+      <c r="V51" s="192"/>
+      <c r="W51" s="193"/>
       <c r="X51" s="9"/>
       <c r="Y51" s="9"/>
     </row>
     <row r="52" ht="22.5" customHeight="1">
       <c r="A52" s="19" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B52" s="19"/>
       <c r="C52" s="19"/>
       <c r="D52" s="19"/>
       <c r="E52" s="19"/>
-      <c r="F52" s="195">
+      <c r="F52" s="194">
         <v>0</v>
       </c>
-      <c r="G52" s="196"/>
-      <c r="H52" s="196"/>
-      <c r="I52" s="196"/>
-      <c r="J52" s="196"/>
-      <c r="K52" s="196"/>
-      <c r="L52" s="196"/>
-      <c r="M52" s="196"/>
-      <c r="N52" s="196"/>
-      <c r="O52" s="196"/>
-      <c r="P52" s="196"/>
-      <c r="Q52" s="196"/>
-      <c r="R52" s="196"/>
-      <c r="S52" s="196"/>
-      <c r="T52" s="196"/>
-      <c r="U52" s="196"/>
-      <c r="V52" s="196"/>
-      <c r="W52" s="197"/>
+      <c r="G52" s="195"/>
+      <c r="H52" s="195"/>
+      <c r="I52" s="195"/>
+      <c r="J52" s="195"/>
+      <c r="K52" s="195"/>
+      <c r="L52" s="195"/>
+      <c r="M52" s="195"/>
+      <c r="N52" s="195"/>
+      <c r="O52" s="195"/>
+      <c r="P52" s="195"/>
+      <c r="Q52" s="195"/>
+      <c r="R52" s="195"/>
+      <c r="S52" s="195"/>
+      <c r="T52" s="195"/>
+      <c r="U52" s="195"/>
+      <c r="V52" s="195"/>
+      <c r="W52" s="196"/>
       <c r="X52" s="9"/>
       <c r="Y52" s="9"/>
     </row>
     <row r="53" ht="22.5" customHeight="1">
       <c r="A53" s="19" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B53" s="19"/>
       <c r="C53" s="19"/>
       <c r="D53" s="19"/>
-      <c r="E53" s="139"/>
-      <c r="F53" s="195">
+      <c r="E53" s="138"/>
+      <c r="F53" s="194">
         <v>0</v>
       </c>
-      <c r="G53" s="196"/>
-      <c r="H53" s="196"/>
-      <c r="I53" s="196"/>
-      <c r="J53" s="196"/>
-      <c r="K53" s="196"/>
-      <c r="L53" s="196"/>
-      <c r="M53" s="196"/>
-      <c r="N53" s="196"/>
-      <c r="O53" s="196"/>
-      <c r="P53" s="196"/>
-      <c r="Q53" s="196"/>
-      <c r="R53" s="196"/>
-      <c r="S53" s="196"/>
-      <c r="T53" s="196"/>
-      <c r="U53" s="196"/>
-      <c r="V53" s="196"/>
-      <c r="W53" s="197"/>
+      <c r="G53" s="195"/>
+      <c r="H53" s="195"/>
+      <c r="I53" s="195"/>
+      <c r="J53" s="195"/>
+      <c r="K53" s="195"/>
+      <c r="L53" s="195"/>
+      <c r="M53" s="195"/>
+      <c r="N53" s="195"/>
+      <c r="O53" s="195"/>
+      <c r="P53" s="195"/>
+      <c r="Q53" s="195"/>
+      <c r="R53" s="195"/>
+      <c r="S53" s="195"/>
+      <c r="T53" s="195"/>
+      <c r="U53" s="195"/>
+      <c r="V53" s="195"/>
+      <c r="W53" s="196"/>
       <c r="X53" s="9"/>
       <c r="Y53" s="9"/>
     </row>
     <row r="54" ht="22.5" customHeight="1">
       <c r="A54" s="19" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B54" s="19"/>
       <c r="C54" s="19"/>
       <c r="D54" s="19"/>
-      <c r="E54" s="139"/>
-      <c r="F54" s="195">
+      <c r="E54" s="138"/>
+      <c r="F54" s="194">
         <v>0</v>
       </c>
-      <c r="G54" s="196"/>
-      <c r="H54" s="196"/>
-      <c r="I54" s="196"/>
-      <c r="J54" s="196"/>
-      <c r="K54" s="196"/>
-      <c r="L54" s="196"/>
-      <c r="M54" s="196"/>
-      <c r="N54" s="196"/>
-      <c r="O54" s="196"/>
-      <c r="P54" s="196"/>
-      <c r="Q54" s="196"/>
-      <c r="R54" s="196"/>
-      <c r="S54" s="196"/>
-      <c r="T54" s="196"/>
-      <c r="U54" s="196"/>
-      <c r="V54" s="196"/>
-      <c r="W54" s="197"/>
+      <c r="G54" s="195"/>
+      <c r="H54" s="195"/>
+      <c r="I54" s="195"/>
+      <c r="J54" s="195"/>
+      <c r="K54" s="195"/>
+      <c r="L54" s="195"/>
+      <c r="M54" s="195"/>
+      <c r="N54" s="195"/>
+      <c r="O54" s="195"/>
+      <c r="P54" s="195"/>
+      <c r="Q54" s="195"/>
+      <c r="R54" s="195"/>
+      <c r="S54" s="195"/>
+      <c r="T54" s="195"/>
+      <c r="U54" s="195"/>
+      <c r="V54" s="195"/>
+      <c r="W54" s="196"/>
       <c r="X54" s="9"/>
       <c r="Y54" s="9"/>
     </row>
     <row r="55" ht="22.5" customHeight="1">
       <c r="A55" s="19" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B55" s="19"/>
       <c r="C55" s="19"/>
       <c r="D55" s="19"/>
-      <c r="E55" s="139"/>
-      <c r="F55" s="195">
+      <c r="E55" s="138"/>
+      <c r="F55" s="194">
         <f>+((F52+F53)*3)</f>
         <v>0</v>
       </c>
-      <c r="G55" s="196"/>
-      <c r="H55" s="196"/>
-      <c r="I55" s="196"/>
-      <c r="J55" s="196"/>
-      <c r="K55" s="196"/>
-      <c r="L55" s="196"/>
-      <c r="M55" s="196">
+      <c r="G55" s="195"/>
+      <c r="H55" s="195"/>
+      <c r="I55" s="195"/>
+      <c r="J55" s="195"/>
+      <c r="K55" s="195"/>
+      <c r="L55" s="195"/>
+      <c r="M55" s="195">
         <f>+F55-F54</f>
         <v>0</v>
       </c>
-      <c r="N55" s="196"/>
-      <c r="O55" s="196"/>
-      <c r="P55" s="196"/>
-      <c r="Q55" s="196"/>
-      <c r="R55" s="196"/>
-      <c r="S55" s="196"/>
-      <c r="T55" s="196"/>
-      <c r="U55" s="196"/>
-      <c r="V55" s="196"/>
-      <c r="W55" s="197"/>
+      <c r="N55" s="195"/>
+      <c r="O55" s="195"/>
+      <c r="P55" s="195"/>
+      <c r="Q55" s="195"/>
+      <c r="R55" s="195"/>
+      <c r="S55" s="195"/>
+      <c r="T55" s="195"/>
+      <c r="U55" s="195"/>
+      <c r="V55" s="195"/>
+      <c r="W55" s="196"/>
       <c r="X55" s="9"/>
       <c r="Y55" s="9"/>
     </row>
     <row r="56" ht="22.5" customHeight="1">
-      <c r="A56" s="198" t="s">
-        <v>112</v>
-      </c>
-      <c r="B56" s="198"/>
-      <c r="C56" s="198"/>
-      <c r="D56" s="198"/>
-      <c r="E56" s="149"/>
-      <c r="F56" s="195">
+      <c r="A56" s="197" t="s">
+        <v>111</v>
+      </c>
+      <c r="B56" s="197"/>
+      <c r="C56" s="197"/>
+      <c r="D56" s="197"/>
+      <c r="E56" s="148"/>
+      <c r="F56" s="194">
         <v>0</v>
       </c>
-      <c r="G56" s="196"/>
-      <c r="H56" s="196"/>
-      <c r="I56" s="196"/>
-      <c r="J56" s="196"/>
-      <c r="K56" s="196"/>
-      <c r="L56" s="196"/>
-      <c r="M56" s="196"/>
-      <c r="N56" s="196"/>
-      <c r="O56" s="196"/>
-      <c r="P56" s="196"/>
-      <c r="Q56" s="196"/>
-      <c r="R56" s="196"/>
-      <c r="S56" s="196"/>
-      <c r="T56" s="196"/>
-      <c r="U56" s="196"/>
-      <c r="V56" s="196"/>
-      <c r="W56" s="197"/>
+      <c r="G56" s="195"/>
+      <c r="H56" s="195"/>
+      <c r="I56" s="195"/>
+      <c r="J56" s="195"/>
+      <c r="K56" s="195"/>
+      <c r="L56" s="195"/>
+      <c r="M56" s="195"/>
+      <c r="N56" s="195"/>
+      <c r="O56" s="195"/>
+      <c r="P56" s="195"/>
+      <c r="Q56" s="195"/>
+      <c r="R56" s="195"/>
+      <c r="S56" s="195"/>
+      <c r="T56" s="195"/>
+      <c r="U56" s="195"/>
+      <c r="V56" s="195"/>
+      <c r="W56" s="196"/>
       <c r="X56" s="9"/>
       <c r="Y56" s="9"/>
     </row>
     <row r="57" ht="22.5" customHeight="1">
-      <c r="A57" s="139" t="s">
+      <c r="A57" s="138" t="s">
+        <v>112</v>
+      </c>
+      <c r="B57" s="143"/>
+      <c r="C57" s="143"/>
+      <c r="D57" s="139"/>
+      <c r="E57" s="144"/>
+      <c r="F57" s="23" t="s">
         <v>113</v>
-      </c>
-      <c r="B57" s="144"/>
-      <c r="C57" s="144"/>
-      <c r="D57" s="140"/>
-      <c r="E57" s="145"/>
-      <c r="F57" s="23" t="s">
-        <v>114</v>
       </c>
       <c r="G57" s="24"/>
       <c r="H57" s="24"/>
       <c r="I57" s="25"/>
       <c r="J57" s="44"/>
       <c r="K57" s="23" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="L57" s="24"/>
       <c r="M57" s="24"/>
@@ -3889,43 +3852,43 @@
       <c r="O57" s="25"/>
       <c r="P57" s="44"/>
       <c r="Q57" s="23" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="R57" s="24"/>
       <c r="S57" s="24"/>
       <c r="T57" s="24"/>
       <c r="U57" s="25"/>
       <c r="V57" s="23"/>
-      <c r="W57" s="199"/>
+      <c r="W57" s="198"/>
       <c r="X57" s="9"/>
       <c r="Y57" s="9"/>
     </row>
     <row r="58" ht="22.5" customHeight="1">
-      <c r="A58" s="200" t="s">
-        <v>117</v>
-      </c>
-      <c r="B58" s="201"/>
-      <c r="C58" s="202"/>
-      <c r="D58" s="203"/>
-      <c r="E58" s="204"/>
-      <c r="F58" s="204"/>
-      <c r="G58" s="204"/>
-      <c r="H58" s="204"/>
-      <c r="I58" s="204"/>
-      <c r="J58" s="204"/>
-      <c r="K58" s="204"/>
-      <c r="L58" s="204"/>
-      <c r="M58" s="204"/>
-      <c r="N58" s="204"/>
-      <c r="O58" s="204"/>
-      <c r="P58" s="204"/>
-      <c r="Q58" s="204"/>
-      <c r="R58" s="204"/>
-      <c r="S58" s="204"/>
-      <c r="T58" s="204"/>
-      <c r="U58" s="204"/>
-      <c r="V58" s="204"/>
-      <c r="W58" s="205"/>
+      <c r="A58" s="199" t="s">
+        <v>116</v>
+      </c>
+      <c r="B58" s="200"/>
+      <c r="C58" s="201"/>
+      <c r="D58" s="202"/>
+      <c r="E58" s="203"/>
+      <c r="F58" s="203"/>
+      <c r="G58" s="203"/>
+      <c r="H58" s="203"/>
+      <c r="I58" s="203"/>
+      <c r="J58" s="203"/>
+      <c r="K58" s="203"/>
+      <c r="L58" s="203"/>
+      <c r="M58" s="203"/>
+      <c r="N58" s="203"/>
+      <c r="O58" s="203"/>
+      <c r="P58" s="203"/>
+      <c r="Q58" s="203"/>
+      <c r="R58" s="203"/>
+      <c r="S58" s="203"/>
+      <c r="T58" s="203"/>
+      <c r="U58" s="203"/>
+      <c r="V58" s="203"/>
+      <c r="W58" s="204"/>
       <c r="X58" s="9"/>
       <c r="Y58" s="9"/>
     </row>
@@ -3934,25 +3897,25 @@
       <c r="B59" s="24"/>
       <c r="C59" s="24"/>
       <c r="D59" s="24"/>
-      <c r="E59" s="118"/>
-      <c r="F59" s="118"/>
-      <c r="G59" s="118"/>
-      <c r="H59" s="118"/>
-      <c r="I59" s="118"/>
-      <c r="J59" s="118"/>
-      <c r="K59" s="118"/>
-      <c r="L59" s="118"/>
-      <c r="M59" s="118"/>
-      <c r="N59" s="118"/>
-      <c r="O59" s="118"/>
-      <c r="P59" s="118"/>
-      <c r="Q59" s="118"/>
-      <c r="R59" s="118"/>
-      <c r="S59" s="118"/>
-      <c r="T59" s="118"/>
-      <c r="U59" s="118"/>
-      <c r="V59" s="118"/>
-      <c r="W59" s="119"/>
+      <c r="E59" s="117"/>
+      <c r="F59" s="117"/>
+      <c r="G59" s="117"/>
+      <c r="H59" s="117"/>
+      <c r="I59" s="117"/>
+      <c r="J59" s="117"/>
+      <c r="K59" s="117"/>
+      <c r="L59" s="117"/>
+      <c r="M59" s="117"/>
+      <c r="N59" s="117"/>
+      <c r="O59" s="117"/>
+      <c r="P59" s="117"/>
+      <c r="Q59" s="117"/>
+      <c r="R59" s="117"/>
+      <c r="S59" s="117"/>
+      <c r="T59" s="117"/>
+      <c r="U59" s="117"/>
+      <c r="V59" s="117"/>
+      <c r="W59" s="118"/>
       <c r="X59" s="9"/>
       <c r="Y59" s="9"/>
     </row>
@@ -4011,37 +3974,37 @@
       <c r="Y61" s="9"/>
     </row>
     <row r="62" ht="22.5" customHeight="1">
-      <c r="A62" s="206" t="s">
-        <v>118</v>
-      </c>
-      <c r="B62" s="207"/>
-      <c r="C62" s="207"/>
-      <c r="D62" s="207"/>
-      <c r="E62" s="207"/>
-      <c r="F62" s="207"/>
-      <c r="G62" s="207"/>
-      <c r="H62" s="207"/>
-      <c r="I62" s="207"/>
-      <c r="J62" s="207"/>
-      <c r="K62" s="207"/>
-      <c r="L62" s="207"/>
-      <c r="M62" s="207"/>
-      <c r="N62" s="207"/>
-      <c r="O62" s="207"/>
-      <c r="P62" s="207"/>
-      <c r="Q62" s="207"/>
-      <c r="R62" s="207"/>
-      <c r="S62" s="207"/>
-      <c r="T62" s="207"/>
-      <c r="U62" s="207"/>
-      <c r="V62" s="207"/>
-      <c r="W62" s="208"/>
-      <c r="X62" s="209"/>
-      <c r="Y62" s="209"/>
+      <c r="A62" s="205" t="s">
+        <v>117</v>
+      </c>
+      <c r="B62" s="206"/>
+      <c r="C62" s="206"/>
+      <c r="D62" s="206"/>
+      <c r="E62" s="206"/>
+      <c r="F62" s="206"/>
+      <c r="G62" s="206"/>
+      <c r="H62" s="206"/>
+      <c r="I62" s="206"/>
+      <c r="J62" s="206"/>
+      <c r="K62" s="206"/>
+      <c r="L62" s="206"/>
+      <c r="M62" s="206"/>
+      <c r="N62" s="206"/>
+      <c r="O62" s="206"/>
+      <c r="P62" s="206"/>
+      <c r="Q62" s="206"/>
+      <c r="R62" s="206"/>
+      <c r="S62" s="206"/>
+      <c r="T62" s="206"/>
+      <c r="U62" s="206"/>
+      <c r="V62" s="206"/>
+      <c r="W62" s="207"/>
+      <c r="X62" s="208"/>
+      <c r="Y62" s="208"/>
     </row>
     <row r="63" ht="22.5" customHeight="1">
       <c r="A63" s="19" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B63" s="19"/>
       <c r="C63" s="19"/>
@@ -4056,23 +4019,23 @@
       <c r="L63" s="57"/>
       <c r="M63" s="57"/>
       <c r="N63" s="57"/>
-      <c r="O63" s="210" t="s">
-        <v>120</v>
-      </c>
-      <c r="P63" s="210"/>
-      <c r="Q63" s="210"/>
-      <c r="R63" s="210"/>
-      <c r="S63" s="210"/>
-      <c r="T63" s="210"/>
-      <c r="U63" s="210"/>
-      <c r="V63" s="210"/>
-      <c r="W63" s="210"/>
+      <c r="O63" s="209" t="s">
+        <v>119</v>
+      </c>
+      <c r="P63" s="209"/>
+      <c r="Q63" s="209"/>
+      <c r="R63" s="209"/>
+      <c r="S63" s="209"/>
+      <c r="T63" s="209"/>
+      <c r="U63" s="209"/>
+      <c r="V63" s="209"/>
+      <c r="W63" s="209"/>
       <c r="X63" s="9"/>
       <c r="Y63" s="9"/>
     </row>
     <row r="64" ht="22.5" customHeight="1">
       <c r="A64" s="19" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B64" s="19"/>
       <c r="C64" s="19"/>
@@ -4087,21 +4050,21 @@
       <c r="L64" s="57"/>
       <c r="M64" s="57"/>
       <c r="N64" s="57"/>
-      <c r="O64" s="210"/>
-      <c r="P64" s="210"/>
-      <c r="Q64" s="210"/>
-      <c r="R64" s="210"/>
-      <c r="S64" s="210"/>
-      <c r="T64" s="210"/>
-      <c r="U64" s="210"/>
-      <c r="V64" s="210"/>
-      <c r="W64" s="210"/>
+      <c r="O64" s="209"/>
+      <c r="P64" s="209"/>
+      <c r="Q64" s="209"/>
+      <c r="R64" s="209"/>
+      <c r="S64" s="209"/>
+      <c r="T64" s="209"/>
+      <c r="U64" s="209"/>
+      <c r="V64" s="209"/>
+      <c r="W64" s="209"/>
       <c r="X64" s="9"/>
       <c r="Y64" s="9"/>
     </row>
     <row r="65" ht="22.5" customHeight="1">
       <c r="A65" s="19" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B65" s="19"/>
       <c r="C65" s="19"/>
@@ -4116,21 +4079,21 @@
       <c r="L65" s="57"/>
       <c r="M65" s="57"/>
       <c r="N65" s="57"/>
-      <c r="O65" s="210"/>
-      <c r="P65" s="210"/>
-      <c r="Q65" s="210"/>
-      <c r="R65" s="210"/>
-      <c r="S65" s="210"/>
-      <c r="T65" s="210"/>
-      <c r="U65" s="210"/>
-      <c r="V65" s="210"/>
-      <c r="W65" s="210"/>
+      <c r="O65" s="209"/>
+      <c r="P65" s="209"/>
+      <c r="Q65" s="209"/>
+      <c r="R65" s="209"/>
+      <c r="S65" s="209"/>
+      <c r="T65" s="209"/>
+      <c r="U65" s="209"/>
+      <c r="V65" s="209"/>
+      <c r="W65" s="209"/>
       <c r="X65" s="9"/>
       <c r="Y65" s="9"/>
     </row>
     <row r="66" ht="22.5" customHeight="1">
       <c r="A66" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B66" s="19"/>
       <c r="C66" s="19"/>
@@ -4145,119 +4108,119 @@
       <c r="L66" s="57"/>
       <c r="M66" s="57"/>
       <c r="N66" s="57"/>
-      <c r="O66" s="210"/>
-      <c r="P66" s="210"/>
-      <c r="Q66" s="210"/>
-      <c r="R66" s="210"/>
-      <c r="S66" s="210"/>
-      <c r="T66" s="210"/>
-      <c r="U66" s="210"/>
-      <c r="V66" s="210"/>
-      <c r="W66" s="210"/>
+      <c r="O66" s="209"/>
+      <c r="P66" s="209"/>
+      <c r="Q66" s="209"/>
+      <c r="R66" s="209"/>
+      <c r="S66" s="209"/>
+      <c r="T66" s="209"/>
+      <c r="U66" s="209"/>
+      <c r="V66" s="209"/>
+      <c r="W66" s="209"/>
       <c r="X66" s="9"/>
       <c r="Y66" s="9"/>
     </row>
     <row r="67" ht="15" customHeight="1">
-      <c r="A67" s="211"/>
-      <c r="B67" s="212"/>
-      <c r="C67" s="212"/>
-      <c r="D67" s="213"/>
-      <c r="E67" s="211"/>
-      <c r="F67" s="212"/>
-      <c r="G67" s="212"/>
-      <c r="H67" s="212"/>
-      <c r="I67" s="213"/>
-      <c r="J67" s="211"/>
-      <c r="K67" s="212"/>
-      <c r="L67" s="212"/>
-      <c r="M67" s="212"/>
-      <c r="N67" s="213"/>
-      <c r="O67" s="214" t="s">
-        <v>124</v>
-      </c>
-      <c r="P67" s="215"/>
-      <c r="Q67" s="215"/>
-      <c r="R67" s="215"/>
-      <c r="S67" s="215"/>
-      <c r="T67" s="215"/>
-      <c r="U67" s="215"/>
-      <c r="V67" s="215"/>
-      <c r="W67" s="216"/>
+      <c r="A67" s="210"/>
+      <c r="B67" s="211"/>
+      <c r="C67" s="211"/>
+      <c r="D67" s="212"/>
+      <c r="E67" s="210"/>
+      <c r="F67" s="211"/>
+      <c r="G67" s="211"/>
+      <c r="H67" s="211"/>
+      <c r="I67" s="212"/>
+      <c r="J67" s="210"/>
+      <c r="K67" s="211"/>
+      <c r="L67" s="211"/>
+      <c r="M67" s="211"/>
+      <c r="N67" s="212"/>
+      <c r="O67" s="213" t="s">
+        <v>123</v>
+      </c>
+      <c r="P67" s="214"/>
+      <c r="Q67" s="214"/>
+      <c r="R67" s="214"/>
+      <c r="S67" s="214"/>
+      <c r="T67" s="214"/>
+      <c r="U67" s="214"/>
+      <c r="V67" s="214"/>
+      <c r="W67" s="215"/>
       <c r="X67" s="9"/>
       <c r="Y67" s="9"/>
     </row>
     <row r="68" ht="30.75" customHeight="1">
-      <c r="A68" s="217"/>
-      <c r="B68" s="218"/>
-      <c r="C68" s="218"/>
-      <c r="D68" s="219"/>
-      <c r="E68" s="217"/>
-      <c r="F68" s="218"/>
-      <c r="G68" s="218"/>
-      <c r="H68" s="218"/>
-      <c r="I68" s="219"/>
-      <c r="J68" s="217"/>
-      <c r="K68" s="218"/>
-      <c r="L68" s="218"/>
-      <c r="M68" s="218"/>
-      <c r="N68" s="219"/>
-      <c r="O68" s="220"/>
-      <c r="P68" s="221"/>
-      <c r="Q68" s="221"/>
-      <c r="R68" s="221"/>
-      <c r="S68" s="221"/>
-      <c r="T68" s="221"/>
-      <c r="U68" s="221"/>
-      <c r="V68" s="221"/>
-      <c r="W68" s="222"/>
+      <c r="A68" s="216"/>
+      <c r="B68" s="217"/>
+      <c r="C68" s="217"/>
+      <c r="D68" s="218"/>
+      <c r="E68" s="216"/>
+      <c r="F68" s="217"/>
+      <c r="G68" s="217"/>
+      <c r="H68" s="217"/>
+      <c r="I68" s="218"/>
+      <c r="J68" s="216"/>
+      <c r="K68" s="217"/>
+      <c r="L68" s="217"/>
+      <c r="M68" s="217"/>
+      <c r="N68" s="218"/>
+      <c r="O68" s="219"/>
+      <c r="P68" s="220"/>
+      <c r="Q68" s="220"/>
+      <c r="R68" s="220"/>
+      <c r="S68" s="220"/>
+      <c r="T68" s="220"/>
+      <c r="U68" s="220"/>
+      <c r="V68" s="220"/>
+      <c r="W68" s="221"/>
       <c r="X68" s="9"/>
       <c r="Y68" s="9"/>
     </row>
     <row r="69" ht="114" customHeight="1">
-      <c r="A69" s="217"/>
-      <c r="B69" s="218"/>
-      <c r="C69" s="218"/>
-      <c r="D69" s="219"/>
-      <c r="E69" s="217"/>
-      <c r="F69" s="218"/>
-      <c r="G69" s="218"/>
-      <c r="H69" s="218"/>
-      <c r="I69" s="219"/>
-      <c r="J69" s="217"/>
-      <c r="K69" s="218"/>
-      <c r="L69" s="218"/>
-      <c r="M69" s="218"/>
-      <c r="N69" s="219"/>
-      <c r="O69" s="223" t="s">
-        <v>125</v>
-      </c>
-      <c r="P69" s="224"/>
-      <c r="Q69" s="224"/>
-      <c r="R69" s="224"/>
-      <c r="S69" s="224"/>
-      <c r="T69" s="224"/>
-      <c r="U69" s="224"/>
-      <c r="V69" s="224"/>
-      <c r="W69" s="225"/>
+      <c r="A69" s="216"/>
+      <c r="B69" s="217"/>
+      <c r="C69" s="217"/>
+      <c r="D69" s="218"/>
+      <c r="E69" s="216"/>
+      <c r="F69" s="217"/>
+      <c r="G69" s="217"/>
+      <c r="H69" s="217"/>
+      <c r="I69" s="218"/>
+      <c r="J69" s="216"/>
+      <c r="K69" s="217"/>
+      <c r="L69" s="217"/>
+      <c r="M69" s="217"/>
+      <c r="N69" s="218"/>
+      <c r="O69" s="222" t="s">
+        <v>124</v>
+      </c>
+      <c r="P69" s="223"/>
+      <c r="Q69" s="223"/>
+      <c r="R69" s="223"/>
+      <c r="S69" s="223"/>
+      <c r="T69" s="223"/>
+      <c r="U69" s="223"/>
+      <c r="V69" s="223"/>
+      <c r="W69" s="224"/>
       <c r="X69" s="9"/>
       <c r="Y69" s="9"/>
     </row>
     <row r="70" ht="18" customHeight="1">
-      <c r="A70" s="217"/>
-      <c r="B70" s="218"/>
-      <c r="C70" s="218"/>
-      <c r="D70" s="219"/>
-      <c r="E70" s="217"/>
-      <c r="F70" s="218"/>
-      <c r="G70" s="218"/>
-      <c r="H70" s="218"/>
-      <c r="I70" s="219"/>
-      <c r="J70" s="217"/>
-      <c r="K70" s="218"/>
-      <c r="L70" s="218"/>
-      <c r="M70" s="218"/>
-      <c r="N70" s="219"/>
-      <c r="O70" s="223">
+      <c r="A70" s="216"/>
+      <c r="B70" s="217"/>
+      <c r="C70" s="217"/>
+      <c r="D70" s="218"/>
+      <c r="E70" s="216"/>
+      <c r="F70" s="217"/>
+      <c r="G70" s="217"/>
+      <c r="H70" s="217"/>
+      <c r="I70" s="218"/>
+      <c r="J70" s="216"/>
+      <c r="K70" s="217"/>
+      <c r="L70" s="217"/>
+      <c r="M70" s="217"/>
+      <c r="N70" s="218"/>
+      <c r="O70" s="222">
         <f>+C11</f>
         <v>0</v>
       </c>
@@ -4268,72 +4231,72 @@
       <c r="T70" s="9"/>
       <c r="U70" s="9"/>
       <c r="V70" s="9"/>
-      <c r="W70" s="226"/>
-      <c r="X70" s="227"/>
-      <c r="Y70" s="228"/>
+      <c r="W70" s="225"/>
+      <c r="X70" s="226"/>
+      <c r="Y70" s="227"/>
     </row>
     <row r="71" ht="13.5" customHeight="1">
-      <c r="A71" s="229" t="s">
+      <c r="A71" s="228" t="s">
+        <v>125</v>
+      </c>
+      <c r="B71" s="229"/>
+      <c r="C71" s="229"/>
+      <c r="D71" s="230"/>
+      <c r="E71" s="228" t="s">
+        <v>125</v>
+      </c>
+      <c r="F71" s="229"/>
+      <c r="G71" s="229"/>
+      <c r="H71" s="229"/>
+      <c r="I71" s="230"/>
+      <c r="J71" s="228" t="s">
+        <v>125</v>
+      </c>
+      <c r="K71" s="229"/>
+      <c r="L71" s="229"/>
+      <c r="M71" s="229"/>
+      <c r="N71" s="230"/>
+      <c r="O71" s="231" t="s">
         <v>126</v>
       </c>
-      <c r="B71" s="230"/>
-      <c r="C71" s="230"/>
-      <c r="D71" s="231"/>
-      <c r="E71" s="229" t="s">
-        <v>126</v>
-      </c>
-      <c r="F71" s="230"/>
-      <c r="G71" s="230"/>
-      <c r="H71" s="230"/>
-      <c r="I71" s="231"/>
-      <c r="J71" s="229" t="s">
-        <v>126</v>
-      </c>
-      <c r="K71" s="230"/>
-      <c r="L71" s="230"/>
-      <c r="M71" s="230"/>
-      <c r="N71" s="231"/>
-      <c r="O71" s="232" t="s">
-        <v>127</v>
-      </c>
-      <c r="P71" s="233">
+      <c r="P71" s="232">
         <f>+A13</f>
         <v>0</v>
       </c>
-      <c r="Q71" s="233"/>
-      <c r="R71" s="233"/>
-      <c r="S71" s="233"/>
-      <c r="T71" s="233"/>
-      <c r="U71" s="233"/>
-      <c r="V71" s="224"/>
-      <c r="W71" s="225"/>
+      <c r="Q71" s="232"/>
+      <c r="R71" s="232"/>
+      <c r="S71" s="232"/>
+      <c r="T71" s="232"/>
+      <c r="U71" s="232"/>
+      <c r="V71" s="223"/>
+      <c r="W71" s="224"/>
       <c r="X71" s="9"/>
       <c r="Y71" s="9"/>
     </row>
     <row r="72" ht="15.75" customHeight="1">
-      <c r="A72" s="232"/>
-      <c r="B72" s="224"/>
-      <c r="C72" s="224"/>
-      <c r="D72" s="224"/>
-      <c r="E72" s="224"/>
-      <c r="F72" s="224"/>
-      <c r="G72" s="224"/>
-      <c r="H72" s="224"/>
-      <c r="I72" s="224"/>
-      <c r="J72" s="224"/>
-      <c r="K72" s="224"/>
-      <c r="L72" s="224"/>
-      <c r="M72" s="224"/>
-      <c r="N72" s="224"/>
-      <c r="O72" s="224"/>
-      <c r="P72" s="224"/>
-      <c r="Q72" s="224"/>
-      <c r="R72" s="224"/>
-      <c r="S72" s="224"/>
-      <c r="T72" s="224"/>
-      <c r="U72" s="224"/>
-      <c r="V72" s="224"/>
-      <c r="W72" s="225"/>
+      <c r="A72" s="231"/>
+      <c r="B72" s="223"/>
+      <c r="C72" s="223"/>
+      <c r="D72" s="223"/>
+      <c r="E72" s="223"/>
+      <c r="F72" s="223"/>
+      <c r="G72" s="223"/>
+      <c r="H72" s="223"/>
+      <c r="I72" s="223"/>
+      <c r="J72" s="223"/>
+      <c r="K72" s="223"/>
+      <c r="L72" s="223"/>
+      <c r="M72" s="223"/>
+      <c r="N72" s="223"/>
+      <c r="O72" s="223"/>
+      <c r="P72" s="223"/>
+      <c r="Q72" s="223"/>
+      <c r="R72" s="223"/>
+      <c r="S72" s="223"/>
+      <c r="T72" s="223"/>
+      <c r="U72" s="223"/>
+      <c r="V72" s="223"/>
+      <c r="W72" s="224"/>
       <c r="X72" s="9"/>
       <c r="Y72" s="9"/>
     </row>
@@ -4552,7 +4515,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1" disablePrompts="0">
-        <x14:dataValidation xr:uid="{00E300F3-00BE-48C5-AD97-006F00C2001F}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00E90047-0020-439C-AE17-008700E90041}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>"LINEAS DE CRÉDITO,LIBRE INVERSION,EXTRAORDINARIO,CONSUMO,VIVIENDA,CREDIAGIL,CREDIFACIL,VEHICULO,EDUCATIVO,ORDINARIO,VACACIONAL,AGIL,CALAMIDAD"</xm:f>
           </x14:formula1>

</xml_diff>